<commit_message>
Get Data Modif - added manuel key secret field.
</commit_message>
<xml_diff>
--- a/Neural Network for Finance/BTCUSDTW.xlsx
+++ b/Neural Network for Finance/BTCUSDTW.xlsx
@@ -15835,12 +15835,12 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>23917.51000000</t>
+          <t>23944.73000000</t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>139486.36440000</t>
+          <t>146796.62286000</t>
         </is>
       </c>
       <c r="H262" t="n">
@@ -15848,20 +15848,20 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>3327031772.95513470</t>
+          <t>3501756174.58078670</t>
         </is>
       </c>
       <c r="J262" t="n">
-        <v>4873875</v>
+        <v>5150048</v>
       </c>
       <c r="K262" t="inlineStr">
         <is>
-          <t>70427.79463000</t>
+          <t>74088.96360000</t>
         </is>
       </c>
       <c r="L262" t="inlineStr">
         <is>
-          <t>1679828832.85337710</t>
+          <t>1767343752.10381690</t>
         </is>
       </c>
       <c r="M262" t="inlineStr">

</xml_diff>